<commit_message>
presentation 1 nicely done
</commit_message>
<xml_diff>
--- a/data/output/tradeoff/analysis.xlsx
+++ b/data/output/tradeoff/analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yasht\Code\FinalYearProject\data\output\tradeoff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86FED17-91E2-4E93-9211-80449AF52F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6357D8DF-2D6F-4C4F-8F4D-E80C4F047661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,13 +57,13 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>Topsis increased cost by 10%</t>
-  </si>
-  <si>
     <t>CE</t>
   </si>
   <si>
-    <t>but TOPSIS got 54% reduction in total CE over the years</t>
+    <t>Topsis decreased cost by 16%</t>
+  </si>
+  <si>
+    <t>but TOPSIS got 56% reduction in total CE over the years</t>
   </si>
 </sst>
 </file>
@@ -390,7 +390,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,19 +441,19 @@
         <v>2023</v>
       </c>
       <c r="B3">
-        <v>4233580.62802104</v>
+        <v>4115709</v>
       </c>
       <c r="C3">
-        <v>103273194.973437</v>
+        <v>102554683</v>
       </c>
       <c r="E3">
         <v>2023</v>
       </c>
       <c r="F3">
-        <v>4049684.3544789599</v>
+        <v>4507764</v>
       </c>
       <c r="G3">
-        <v>109510223.985871</v>
+        <v>108503834</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -461,19 +461,19 @@
         <v>2024</v>
       </c>
       <c r="B4">
-        <v>4376725.7453051498</v>
+        <v>3610891</v>
       </c>
       <c r="C4">
-        <v>109551495.09485</v>
+        <v>41626621</v>
       </c>
       <c r="E4">
         <v>2024</v>
       </c>
       <c r="F4">
-        <v>4430761.6087809196</v>
+        <v>4358954</v>
       </c>
       <c r="G4">
-        <v>114492517.79628401</v>
+        <v>74426573</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -481,19 +481,19 @@
         <v>2025</v>
       </c>
       <c r="B5">
-        <v>4844502.9607190201</v>
+        <v>3257979</v>
       </c>
       <c r="C5">
-        <v>109952771.13235199</v>
+        <v>72636868</v>
       </c>
       <c r="E5">
         <v>2025</v>
       </c>
       <c r="F5">
-        <v>4929951.7244515503</v>
+        <v>4284770</v>
       </c>
       <c r="G5">
-        <v>118341778.34073099</v>
+        <v>34509109</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -501,19 +501,19 @@
         <v>2026</v>
       </c>
       <c r="B6">
-        <v>6097614.1751269298</v>
+        <v>3541365</v>
       </c>
       <c r="C6">
-        <v>103332354.39698</v>
+        <v>49609096</v>
       </c>
       <c r="E6">
         <v>2026</v>
       </c>
       <c r="F6">
-        <v>5001134.9322967697</v>
+        <v>5389524</v>
       </c>
       <c r="G6">
-        <v>124586570.300981</v>
+        <v>95089672</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -521,19 +521,19 @@
         <v>2027</v>
       </c>
       <c r="B7">
-        <v>5177986.1845187396</v>
+        <v>3874720</v>
       </c>
       <c r="C7">
-        <v>113314609.69960999</v>
+        <v>69924314</v>
       </c>
       <c r="E7">
         <v>2027</v>
       </c>
       <c r="F7">
-        <v>5571632.9013444502</v>
+        <v>5101151</v>
       </c>
       <c r="G7">
-        <v>120834199.31305701</v>
+        <v>61715280</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -541,19 +541,19 @@
         <v>2028</v>
       </c>
       <c r="B8">
-        <v>6132892.3982621003</v>
+        <v>4352695</v>
       </c>
       <c r="C8">
-        <v>108483196.489912</v>
+        <v>31844686</v>
       </c>
       <c r="E8">
         <v>2028</v>
       </c>
       <c r="F8">
-        <v>5698212.4883717801</v>
+        <v>4960658</v>
       </c>
       <c r="G8">
-        <v>134141708.255586</v>
+        <v>54521452</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -561,19 +561,19 @@
         <v>2029</v>
       </c>
       <c r="B9">
-        <v>6332805.2349472595</v>
+        <v>4254041</v>
       </c>
       <c r="C9">
-        <v>107872713.181392</v>
+        <v>53078409</v>
       </c>
       <c r="E9">
         <v>2029</v>
       </c>
       <c r="F9">
-        <v>5707404.3819433097</v>
+        <v>5289381</v>
       </c>
       <c r="G9">
-        <v>137009388.14436799</v>
+        <v>77853687</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -581,19 +581,19 @@
         <v>2030</v>
       </c>
       <c r="B10">
-        <v>6573426.9375380902</v>
+        <v>3867912</v>
       </c>
       <c r="C10">
-        <v>84082435.181471795</v>
+        <v>40875395</v>
       </c>
       <c r="E10">
         <v>2030</v>
       </c>
       <c r="F10">
-        <v>5943963.6409164201</v>
+        <v>4857609</v>
       </c>
       <c r="G10">
-        <v>141398732.598575</v>
+        <v>61853346</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -601,19 +601,19 @@
         <v>2031</v>
       </c>
       <c r="B11">
-        <v>6971727.9674400799</v>
+        <v>4717384</v>
       </c>
       <c r="C11">
-        <v>88050797.209850401</v>
+        <v>47643565</v>
       </c>
       <c r="E11">
         <v>2031</v>
       </c>
       <c r="F11">
-        <v>6403273.22377807</v>
+        <v>6295486</v>
       </c>
       <c r="G11">
-        <v>149295697.813178</v>
+        <v>111963711</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -621,19 +621,19 @@
         <v>2032</v>
       </c>
       <c r="B12">
-        <v>7219249.1350616999</v>
+        <v>4997564</v>
       </c>
       <c r="C12">
-        <v>83571552.791854307</v>
+        <v>29411067</v>
       </c>
       <c r="E12">
         <v>2032</v>
       </c>
       <c r="F12">
-        <v>6081274.80601478</v>
+        <v>5180814</v>
       </c>
       <c r="G12">
-        <v>147858811.62912101</v>
+        <v>54556791</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -641,19 +641,19 @@
         <v>2033</v>
       </c>
       <c r="B13">
-        <v>8412870.5829924904</v>
+        <v>5715050</v>
       </c>
       <c r="C13">
-        <v>68945297.859952301</v>
+        <v>41315167</v>
       </c>
       <c r="E13">
         <v>2033</v>
       </c>
       <c r="F13">
-        <v>6374013.7904898496</v>
+        <v>6746906</v>
       </c>
       <c r="G13">
-        <v>114414948.625626</v>
+        <v>115129283</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -661,19 +661,19 @@
         <v>2034</v>
       </c>
       <c r="B14">
-        <v>8539624.0148971695</v>
+        <v>4389765</v>
       </c>
       <c r="C14">
-        <v>69986876.520834103</v>
+        <v>28956417</v>
       </c>
       <c r="E14">
         <v>2034</v>
       </c>
       <c r="F14">
-        <v>6540319.6404739702</v>
+        <v>5682924</v>
       </c>
       <c r="G14">
-        <v>180019234.36653799</v>
+        <v>77300851</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -681,19 +681,19 @@
         <v>2035</v>
       </c>
       <c r="B15">
-        <v>8476182.3886578791</v>
+        <v>5385026</v>
       </c>
       <c r="C15">
-        <v>72727374.388890997</v>
+        <v>46170317</v>
       </c>
       <c r="E15">
         <v>2035</v>
       </c>
       <c r="F15">
-        <v>6710720.3870556001</v>
+        <v>6093110</v>
       </c>
       <c r="G15">
-        <v>173962382.68713501</v>
+        <v>76329555</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -701,19 +701,19 @@
         <v>2036</v>
       </c>
       <c r="B16">
-        <v>8637217.9468708597</v>
+        <v>4989551</v>
       </c>
       <c r="C16">
-        <v>74443519.572885796</v>
+        <v>30004642</v>
       </c>
       <c r="E16">
         <v>2036</v>
       </c>
       <c r="F16">
-        <v>7034666.4042578898</v>
+        <v>6938642</v>
       </c>
       <c r="G16">
-        <v>167359074.91120201</v>
+        <v>138404367</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -721,19 +721,19 @@
         <v>2037</v>
       </c>
       <c r="B17">
-        <v>8671541.0002259109</v>
+        <v>6464877</v>
       </c>
       <c r="C17">
-        <v>84940497.040137395</v>
+        <v>70230229</v>
       </c>
       <c r="E17">
         <v>2037</v>
       </c>
       <c r="F17">
-        <v>7458463.5120064896</v>
+        <v>5248071</v>
       </c>
       <c r="G17">
-        <v>162625311.71789199</v>
+        <v>23414506</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -741,37 +741,37 @@
         <v>2038</v>
       </c>
       <c r="B18">
-        <v>9268885.7506841794</v>
+        <v>4108288</v>
       </c>
       <c r="C18">
-        <v>83513903.584184706</v>
+        <v>25511577</v>
       </c>
       <c r="E18">
         <v>2038</v>
       </c>
       <c r="F18">
-        <v>7826381.4166096104</v>
+        <v>6870702</v>
       </c>
       <c r="G18">
-        <v>167512692.94293201</v>
+        <v>158040286</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>SUM(B2:B18)</f>
-        <v>109966833.05126861</v>
+        <v>71642817</v>
       </c>
       <c r="C20">
         <f>SUM(C3:C18)</f>
-        <v>1466042589.1185946</v>
+        <v>781393053</v>
       </c>
       <c r="F20">
         <f>SUM(F3:F18)</f>
-        <v>95761859.213270426</v>
+        <v>87806466</v>
       </c>
       <c r="G20">
         <f>SUM(G3:G18)</f>
-        <v>2263363273.4290771</v>
+        <v>1323612303</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -788,19 +788,19 @@
       </c>
       <c r="C24">
         <f>((B20-F20)/B20)*100</f>
-        <v>12.917507437333905</v>
+        <v>-22.561436968621713</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25">
         <f>((C20-G20)/C20)*100</f>
-        <v>-54.385915540819511</v>
+        <v>-69.391357898340573</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>

</xml_diff>